<commit_message>
Update survival and maternity data
</commit_message>
<xml_diff>
--- a/data/MATERNITY_DATA.xlsx
+++ b/data/MATERNITY_DATA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="787" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="787" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LITTERS" sheetId="1" r:id="rId1"/>
@@ -5533,7 +5533,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5625,7 +5625,7 @@
         <v>38</v>
       </c>
       <c r="K2" s="1" t="str">
-        <f t="shared" ref="K2:K65" si="1">IF(J2&lt;=12,"CUB",IF(J2&lt;=24,"JUVENILE",IF(J2&lt;=36,"SUBADULT",IF(J2&lt;=48,"ADULT_36_48",IF(J2&lt;=60,"ADULT_48_60",IF(J2&lt;=72,"ADULT_60_72",IF(J2&lt;=84,"ADULT_72_84",IF(J2&gt;84,"ADULT_84","NA"))))))))</f>
+        <f>IF(J2&lt;=12,"CUB",IF(J2&lt;=24,"JUVENILE",IF(J2&lt;=36,"SUBADULT",IF(J2&lt;=48,"ADULT_36_48",IF(J2&lt;=60,"ADULT_48_60",IF(J2&lt;=72,"ADULT_60_72",IF(J2&lt;=84,"ADULT_72_84",IF(J2&gt;84,"ADULT_84","NA"))))))))</f>
         <v>ADULT_36_48</v>
       </c>
       <c r="L2" s="10">
@@ -5665,7 +5665,7 @@
         <v>62</v>
       </c>
       <c r="K3" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K2:K65" si="1">IF(J3&lt;=12,"CUB",IF(J3&lt;=24,"JUVENILE",IF(J3&lt;=36,"SUBADULT",IF(J3&lt;=48,"ADULT_36_48",IF(J3&lt;=60,"ADULT_48_60",IF(J3&lt;=72,"ADULT_60_72",IF(J3&lt;=84,"ADULT_72_84",IF(J3&gt;84,"ADULT_84","NA"))))))))</f>
         <v>ADULT_60_72</v>
       </c>
       <c r="L3" s="10">
@@ -26106,7 +26106,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26170,14 +26170,14 @@
         <v>1.8571428571428572</v>
       </c>
       <c r="G4" s="15">
-        <v>0.36313651960128157</v>
+        <v>0.36313651960128202</v>
       </c>
       <c r="H4" s="15">
         <v>20</v>
       </c>
       <c r="I4" s="27">
         <f>G4/SQRT(H4)</f>
-        <v>8.1199794294115044E-2</v>
+        <v>8.1199794294115141E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>